<commit_message>
Simplify Use case description
</commit_message>
<xml_diff>
--- a/Use case description.xlsx
+++ b/Use case description.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdok1\Documents\Tips for being developer\GDSC community activity\SE-hw2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\SE-hw2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694D3E73-FAC4-4525-9F10-110571CE6DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54691FCB-2927-4F5F-9DDE-25D217C4EED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -79,17 +79,6 @@
  4. 해당 채용의 상세한 정보(회사이름, 업무, 인원수, 신청 마감일)가 출력</t>
   </si>
   <si>
-    <t>1. 사용자가 지원 정보를 선택함
- 3. 사용자가 '지원 취소' 버튼을 클릭함
- 6. 사용자가 지원 취소를 승인함</t>
-  </si>
-  <si>
-    <t>2. 선택한 지원 정보를 강조하여 표시함
- 4. 지원의 마감일을 확인함
- 5.지원 취소 확인 메시지 ("정말로 지원을 취소하시겠습니까?")를 보냄
- 7. 지원을 취소함</t>
-  </si>
-  <si>
     <t>Alternative Courses
  Step 2에서 지원 정보가 없는 경우, '아직 등록한 지원 정보가 없습니다' 메시지를 출력함</t>
   </si>
@@ -101,11 +90,6 @@
     <t>채용 정보 등록 기능</t>
   </si>
   <si>
-    <t>2. 등록한 채용 정보 리스트를 출력
-4. 업무, 인원 수, 신청 마감일 등 정보 입력칸을 보여줌
-6. "채용 정보 등록완료" 메세지 출력</t>
-  </si>
-  <si>
     <t>채용 정보 조회 기능</t>
   </si>
   <si>
@@ -1542,8 +1526,762 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1. None
-3. </t>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>통계</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보기를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선택함</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>통계</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보기를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선택함</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조회</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>버튼을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>클릭함</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반회원이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회사</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원하기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>버튼을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>클릭</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로그</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아웃을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선택한다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로그아웃</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>성공</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>화면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력해준다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 업무별 지원 횟수를 출력함</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 회사 회원이 채용 정보 조회를 선택함</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 회사 회원이 채용 정보 등록을 선택함
+3. 업무, 인원 수, 신청 마감일 등 정보 입력</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>업무</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>인원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>마감일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>입력칸을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보여줌
+4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. "</t>
     </r>
     <r>
       <rPr>
@@ -1591,26 +2329,137 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>등록</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">선택
+      <t>등록완료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>메세지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선택한</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>강조하여</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">표시함
 </t>
     </r>
     <r>
@@ -1620,158 +2469,40 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">5. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>업무</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>인원</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>신청</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>마감일</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>등</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>정보</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>입력</t>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>취소함</t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>1.None</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">1. </t>
     </r>
@@ -1802,89 +2533,55 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>지원자</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>통계</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>보기를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>선택함</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
+      <t>지원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">선택함
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 3. </t>
     </r>
     <r>
       <rPr>
@@ -1903,7 +2600,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> '</t>
     </r>
     <r>
       <rPr>
@@ -1932,137 +2629,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>정보</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>통계</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>보기를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>선택함</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사용자가</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>지원</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>정보</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>조회</t>
+      <t>취소</t>
     </r>
     <r>
       <rPr>
@@ -2102,247 +2669,6 @@
       </rPr>
       <t>클릭함</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>일반회원이</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>회사</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>지원하기</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>버튼을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>클릭</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>로그</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>아웃을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>선택한다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>로그아웃</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>성공</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>화면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>출력해준다</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 업무별 지원 횟수를 출력함</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2350,7 +2676,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2416,6 +2742,20 @@
       <family val="2"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic Semilight"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic Semilight"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2569,7 +2909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2594,6 +2934,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2623,7 +2966,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2846,25 +3192,25 @@
   </sheetPr>
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="56.7265625" customWidth="1"/>
+    <col min="3" max="3" width="56.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.5">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="12.75">
+      <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-    </row>
-    <row r="2" spans="1:3" ht="12.5">
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" ht="12.75">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2876,57 +3222,57 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>27</v>
+      <c r="B3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27.75" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" spans="1:3" ht="28.5" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="33.75" customHeight="1">
+      <c r="A6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="7" spans="1:3" ht="45" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="21"/>
     </row>
     <row r="8" spans="1:3" ht="25.5" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="65.25" customHeight="1">
@@ -2945,7 +3291,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>9</v>
@@ -2956,79 +3302,79 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="40">
+    <row r="12" spans="1:3" ht="22.5">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="12.75">
+      <c r="A13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="33" customHeight="1">
+      <c r="A14" s="11"/>
+      <c r="B14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A16" s="11"/>
+      <c r="B16" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="12.5">
-      <c r="A13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="16" t="s">
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:3" ht="45.95" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="32.25" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" ht="46" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
+      <c r="B17" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="31.5" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>34</v>
+        <v>21</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="43.5" customHeight="1"/>
@@ -3038,66 +3384,66 @@
     <row r="23" spans="1:3" ht="36" customHeight="1"/>
     <row r="24" spans="1:3" ht="48" customHeight="1"/>
     <row r="25" spans="1:3" ht="45" customHeight="1"/>
-    <row r="28" spans="1:3" ht="12.5"/>
-    <row r="29" spans="1:3" ht="12.5"/>
-    <row r="30" spans="1:3" ht="12.5"/>
-    <row r="31" spans="1:3" ht="12.5"/>
-    <row r="32" spans="1:3" ht="12.5"/>
-    <row r="33" ht="12.5"/>
-    <row r="34" ht="12.5"/>
-    <row r="35" ht="12.5"/>
-    <row r="36" ht="12.5"/>
-    <row r="37" ht="12.5"/>
-    <row r="38" ht="12.5"/>
-    <row r="39" ht="12.5"/>
-    <row r="40" ht="12.5"/>
-    <row r="41" ht="12.5"/>
-    <row r="42" ht="12.5"/>
-    <row r="43" ht="12.5"/>
-    <row r="44" ht="12.5"/>
-    <row r="45" ht="12.5"/>
-    <row r="46" ht="12.5"/>
-    <row r="47" ht="12.5"/>
-    <row r="48" ht="12.5"/>
-    <row r="49" ht="12.5"/>
-    <row r="50" ht="12.5"/>
-    <row r="51" ht="12.5"/>
-    <row r="52" ht="12.5"/>
-    <row r="53" ht="12.5"/>
-    <row r="54" ht="12.5"/>
-    <row r="55" ht="12.5"/>
-    <row r="56" ht="12.5"/>
-    <row r="57" ht="12.5"/>
-    <row r="58" ht="12.5"/>
-    <row r="59" ht="12.5"/>
-    <row r="60" ht="12.5"/>
-    <row r="61" ht="12.5"/>
-    <row r="62" ht="12.5"/>
-    <row r="63" ht="12.5"/>
-    <row r="64" ht="12.5"/>
-    <row r="65" ht="12.5"/>
-    <row r="66" ht="12.5"/>
-    <row r="67" ht="12.5"/>
-    <row r="68" ht="12.5"/>
-    <row r="69" ht="12.5"/>
-    <row r="70" ht="12.5"/>
-    <row r="71" ht="12.5"/>
-    <row r="72" ht="12.5"/>
-    <row r="73" ht="12.5"/>
-    <row r="74" ht="12.5"/>
-    <row r="75" ht="12.5"/>
-    <row r="76" ht="12.5"/>
-    <row r="77" ht="12.5"/>
-    <row r="78" ht="12.5"/>
-    <row r="79" ht="12.5"/>
-    <row r="80" ht="12.5"/>
-    <row r="81" ht="12.5"/>
-    <row r="82" ht="12.5"/>
-    <row r="83" ht="12.5"/>
-    <row r="100" spans="4:4" ht="12.5">
+    <row r="28" spans="1:3" ht="12.75"/>
+    <row r="29" spans="1:3" ht="12.75"/>
+    <row r="30" spans="1:3" ht="12.75"/>
+    <row r="31" spans="1:3" ht="12.75"/>
+    <row r="32" spans="1:3" ht="12.75"/>
+    <row r="33" ht="12.75"/>
+    <row r="34" ht="12.75"/>
+    <row r="35" ht="12.75"/>
+    <row r="36" ht="12.75"/>
+    <row r="37" ht="12.75"/>
+    <row r="38" ht="12.75"/>
+    <row r="39" ht="12.75"/>
+    <row r="40" ht="12.75"/>
+    <row r="41" ht="12.75"/>
+    <row r="42" ht="12.75"/>
+    <row r="43" ht="12.75"/>
+    <row r="44" ht="12.75"/>
+    <row r="45" ht="12.75"/>
+    <row r="46" ht="12.75"/>
+    <row r="47" ht="12.75"/>
+    <row r="48" ht="12.75"/>
+    <row r="49" ht="12.75"/>
+    <row r="50" ht="12.75"/>
+    <row r="51" ht="12.75"/>
+    <row r="52" ht="12.75"/>
+    <row r="53" ht="12.75"/>
+    <row r="54" ht="12.75"/>
+    <row r="55" ht="12.75"/>
+    <row r="56" ht="12.75"/>
+    <row r="57" ht="12.75"/>
+    <row r="58" ht="12.75"/>
+    <row r="59" ht="12.75"/>
+    <row r="60" ht="12.75"/>
+    <row r="61" ht="12.75"/>
+    <row r="62" ht="12.75"/>
+    <row r="63" ht="12.75"/>
+    <row r="64" ht="12.75"/>
+    <row r="65" ht="12.75"/>
+    <row r="66" ht="12.75"/>
+    <row r="67" ht="12.75"/>
+    <row r="68" ht="12.75"/>
+    <row r="69" ht="12.75"/>
+    <row r="70" ht="12.75"/>
+    <row r="71" ht="12.75"/>
+    <row r="72" ht="12.75"/>
+    <row r="73" ht="12.75"/>
+    <row r="74" ht="12.75"/>
+    <row r="75" ht="12.75"/>
+    <row r="76" ht="12.75"/>
+    <row r="77" ht="12.75"/>
+    <row r="78" ht="12.75"/>
+    <row r="79" ht="12.75"/>
+    <row r="80" ht="12.75"/>
+    <row r="81" ht="12.75"/>
+    <row r="82" ht="12.75"/>
+    <row r="83" ht="12.75"/>
+    <row r="100" spans="4:4" ht="12.75">
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="4:4" ht="12.5">
+    <row r="101" spans="4:4" ht="12.75">
       <c r="D101" s="1"/>
     </row>
     <row r="102" spans="4:4" ht="48" customHeight="1">

</xml_diff>